<commit_message>
Edit table formats to fit on one page
</commit_message>
<xml_diff>
--- a/Figures-Tables-Manuscript/Manuscript/T1_SETTING-MODERN.xlsx
+++ b/Figures-Tables-Manuscript/Manuscript/T1_SETTING-MODERN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jocelynreahl/Documents/BergmannLab_2018-2020/Reahl_2020/Figures-Tables-Manuscript/Manuscript/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{826F4ACA-85AD-634B-9CF7-CB893E2508C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1A91ACA-2920-7A48-BF03-56C19B2E4FAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="14200" xr2:uid="{1B76908D-EF33-F346-88FB-8F4712C0C3B8}"/>
   </bookViews>
@@ -258,7 +258,7 @@
     <t>12 km Past Tana River Confluence to the Copper River, Alaska, U.S. (CR-24 to CR-41)</t>
   </si>
   <si>
-    <t>Table [SETTING-MODERN]. List of the samples from modern depositional environments considered in this study. Samples are coded by author (letter in parentheses below each sample citation) and number (column '#') for reference in Figure [HEATMAP-MODERN]. Samples from this study are listed individually, while samples from the literature are grouped by sampling location and transport mode. S is the number of samples associated with each entry and N is the total number of quartz grains analyzed per entry.</t>
+    <t>Table 1. List of the samples from modern depositional environments considered in this study. Each group of samples is assigned a number for later reference in Figures 1 and 5 (Column #). Column S indicates the number of samples in each sample group, and column N indicates the number of quartz grains in each sample group.</t>
   </si>
 </sst>
 </file>
@@ -762,17 +762,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0F7B368-73C5-8E46-AE58-54B5A9F73EEF}">
-  <dimension ref="A1:M40"/>
+  <dimension ref="A1:M38"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.33203125" customWidth="1"/>
     <col min="2" max="2" width="3.6640625" customWidth="1"/>
-    <col min="3" max="3" width="38.83203125" customWidth="1"/>
+    <col min="3" max="3" width="31.6640625" customWidth="1"/>
     <col min="4" max="4" width="7.6640625" customWidth="1"/>
     <col min="5" max="6" width="3.6640625" customWidth="1"/>
     <col min="7" max="7" width="19.1640625" customWidth="1"/>
@@ -816,65 +816,100 @@
       <c r="F4" s="29"/>
       <c r="G4" s="29"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="29"/>
-      <c r="B5" s="29"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="29"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="29"/>
-      <c r="B6" s="29"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="29"/>
-      <c r="G6" s="29"/>
-    </row>
-    <row r="7" spans="1:13" ht="8" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="7"/>
-    </row>
-    <row r="8" spans="1:13" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
+    <row r="5" spans="1:13" ht="8" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="7"/>
+    </row>
+    <row r="6" spans="1:13" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B6" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C6" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D6" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E6" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="14" t="s">
+      <c r="F6" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="G8" s="15" t="s">
+      <c r="G6" s="15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="34" t="s">
+    <row r="7" spans="1:13" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="34" t="s">
         <v>27</v>
       </c>
+      <c r="B7" s="16">
+        <v>1</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="17">
+        <v>1</v>
+      </c>
+      <c r="F7" s="17">
+        <v>31</v>
+      </c>
+      <c r="G7" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+    </row>
+    <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="35"/>
+      <c r="B8" s="16">
+        <v>2</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" s="17">
+        <v>1</v>
+      </c>
+      <c r="F8" s="17">
+        <v>34</v>
+      </c>
+      <c r="G8" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="1"/>
+    </row>
+    <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="35"/>
       <c r="B9" s="16">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D9" s="17" t="s">
         <v>0</v>
@@ -883,10 +918,10 @@
         <v>1</v>
       </c>
       <c r="F9" s="17">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G9" s="24" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
@@ -897,10 +932,10 @@
     <row r="10" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="35"/>
       <c r="B10" s="16">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D10" s="17" t="s">
         <v>0</v>
@@ -909,25 +944,24 @@
         <v>1</v>
       </c>
       <c r="F10" s="17">
-        <v>34</v>
-      </c>
-      <c r="G10" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="1"/>
+        <v>44</v>
+      </c>
+      <c r="G10" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="H10" s="9"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
     </row>
     <row r="11" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="35"/>
       <c r="B11" s="16">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D11" s="17" t="s">
         <v>0</v>
@@ -936,76 +970,76 @@
         <v>1</v>
       </c>
       <c r="F11" s="17">
-        <v>30</v>
-      </c>
-      <c r="G11" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
+        <v>48</v>
+      </c>
+      <c r="G11" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="H11" s="9"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
     </row>
     <row r="12" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="35"/>
       <c r="B12" s="16">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E12" s="17">
         <v>1</v>
       </c>
       <c r="F12" s="17">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="G12" s="17" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="H12" s="9"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
     </row>
     <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="35"/>
       <c r="B13" s="16">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E13" s="17">
         <v>1</v>
       </c>
       <c r="F13" s="17">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="G13" s="17" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="H13" s="9"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="8"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
     </row>
     <row r="14" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="35"/>
       <c r="B14" s="16">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D14" s="17" t="s">
         <v>3</v>
@@ -1014,24 +1048,24 @@
         <v>1</v>
       </c>
       <c r="F14" s="17">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="G14" s="17" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="H14" s="9"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
     </row>
     <row r="15" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="35"/>
+      <c r="A15" s="31"/>
       <c r="B15" s="16">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D15" s="17" t="s">
         <v>3</v>
@@ -1040,365 +1074,359 @@
         <v>1</v>
       </c>
       <c r="F15" s="17">
-        <v>39</v>
-      </c>
-      <c r="G15" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="H15" s="9"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
+        <v>40</v>
+      </c>
+      <c r="G15" s="21" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="16" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="35"/>
-      <c r="B16" s="16">
-        <v>8</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="D16" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="E16" s="17">
-        <v>1</v>
-      </c>
-      <c r="F16" s="17">
-        <v>36</v>
-      </c>
-      <c r="G16" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="H16" s="9"/>
+      <c r="A16" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="18">
+        <v>10</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="E16" s="19">
+        <v>5</v>
+      </c>
+      <c r="F16" s="19">
+        <v>250</v>
+      </c>
+      <c r="G16" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="H16" s="3"/>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="2"/>
     </row>
     <row r="17" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="31"/>
+      <c r="A17" s="32"/>
       <c r="B17" s="16">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E17" s="17">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F17" s="17">
-        <v>40</v>
-      </c>
-      <c r="G17" s="21" t="s">
-        <v>45</v>
-      </c>
+        <v>346</v>
+      </c>
+      <c r="G17" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="30" t="s">
-        <v>28</v>
-      </c>
-      <c r="B18" s="18">
-        <v>10</v>
-      </c>
-      <c r="C18" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="E18" s="19">
-        <v>5</v>
-      </c>
-      <c r="F18" s="19">
-        <v>250</v>
-      </c>
-      <c r="G18" s="16" t="s">
-        <v>49</v>
+      <c r="A18" s="32"/>
+      <c r="B18" s="16">
+        <v>12</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" s="17">
+        <v>1</v>
+      </c>
+      <c r="F18" s="17">
+        <v>50</v>
+      </c>
+      <c r="G18" s="27" t="s">
+        <v>50</v>
       </c>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="2"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
     </row>
     <row r="19" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="32"/>
       <c r="B19" s="16">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D19" s="17" t="s">
         <v>2</v>
       </c>
       <c r="E19" s="17">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F19" s="17">
-        <v>346</v>
-      </c>
-      <c r="G19" s="27" t="s">
-        <v>50</v>
+        <v>297</v>
+      </c>
+      <c r="G19" s="16" t="s">
+        <v>51</v>
       </c>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
-      <c r="K19" s="5"/>
-      <c r="L19" s="5"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
     </row>
     <row r="20" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="32"/>
       <c r="B20" s="16">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E20" s="17">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F20" s="17">
-        <v>50</v>
-      </c>
-      <c r="G20" s="27" t="s">
-        <v>50</v>
-      </c>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
+        <v>250</v>
+      </c>
+      <c r="G20" s="28" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="21" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="32"/>
-      <c r="B21" s="16">
-        <v>13</v>
-      </c>
-      <c r="C21" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="D21" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="E21" s="17">
-        <v>6</v>
-      </c>
-      <c r="F21" s="17">
-        <v>297</v>
-      </c>
-      <c r="G21" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
-    </row>
-    <row r="22" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="32"/>
-      <c r="B22" s="16">
-        <v>14</v>
-      </c>
-      <c r="C22" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="D22" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="E22" s="17">
-        <v>5</v>
-      </c>
-      <c r="F22" s="17">
-        <v>250</v>
-      </c>
-      <c r="G22" s="28" t="s">
+      <c r="A21" s="36"/>
+      <c r="B21" s="22">
+        <v>15</v>
+      </c>
+      <c r="C21" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="21">
+        <v>1</v>
+      </c>
+      <c r="F21" s="21">
+        <v>48</v>
+      </c>
+      <c r="G21" s="26" t="s">
         <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" s="18">
+        <v>16</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="D22" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="E22" s="19">
+        <v>3</v>
+      </c>
+      <c r="F22" s="19">
+        <v>60</v>
+      </c>
+      <c r="G22" s="20" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="36"/>
       <c r="B23" s="22">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C23" s="22" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="D23" s="21" t="s">
         <v>3</v>
       </c>
       <c r="E23" s="21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F23" s="21">
-        <v>48</v>
-      </c>
-      <c r="G23" s="26" t="s">
-        <v>52</v>
+        <v>40</v>
+      </c>
+      <c r="G23" s="21" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="30" t="s">
-        <v>29</v>
-      </c>
-      <c r="B24" s="18">
-        <v>16</v>
-      </c>
-      <c r="C24" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" s="16">
+        <v>18</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E24" s="17">
+        <v>22</v>
+      </c>
+      <c r="F24" s="17">
+        <v>626</v>
+      </c>
+      <c r="G24" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="H24" s="10"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
+    </row>
+    <row r="25" spans="1:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="32"/>
+      <c r="B25" s="16">
+        <v>19</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="E25" s="17">
+        <v>18</v>
+      </c>
+      <c r="F25" s="17">
+        <v>450</v>
+      </c>
+      <c r="G25" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="H25" s="12"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+    </row>
+    <row r="26" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" s="18">
+        <v>20</v>
+      </c>
+      <c r="C26" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="E26" s="19">
+        <v>1</v>
+      </c>
+      <c r="F26" s="19">
+        <v>15</v>
+      </c>
+      <c r="G26" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="H26" s="13"/>
+    </row>
+    <row r="27" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="31"/>
+      <c r="B27" s="22">
+        <v>21</v>
+      </c>
+      <c r="C27" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E27" s="21">
+        <v>1</v>
+      </c>
+      <c r="F27" s="21">
+        <v>15</v>
+      </c>
+      <c r="G27" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="H27" s="11"/>
+    </row>
+    <row r="28" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28" s="16">
+        <v>22</v>
+      </c>
+      <c r="C28" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D28" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E28" s="17">
+        <v>1</v>
+      </c>
+      <c r="F28" s="17">
         <v>25</v>
       </c>
-      <c r="D24" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="E24" s="19">
-        <v>3</v>
-      </c>
-      <c r="F24" s="19">
-        <v>60</v>
-      </c>
-      <c r="G24" s="20" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="36"/>
-      <c r="B25" s="22">
-        <v>17</v>
-      </c>
-      <c r="C25" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="D25" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="E25" s="21">
-        <v>2</v>
-      </c>
-      <c r="F25" s="21">
-        <v>40</v>
-      </c>
-      <c r="G25" s="21" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="30" t="s">
-        <v>30</v>
-      </c>
-      <c r="B26" s="16">
-        <v>18</v>
-      </c>
-      <c r="C26" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="D26" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="E26" s="17">
-        <v>22</v>
-      </c>
-      <c r="F26" s="17">
-        <v>626</v>
-      </c>
-      <c r="G26" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="H26" s="10"/>
-      <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
-      <c r="K26" s="5"/>
-      <c r="L26" s="5"/>
-    </row>
-    <row r="27" spans="1:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="32"/>
-      <c r="B27" s="16">
-        <v>19</v>
-      </c>
-      <c r="C27" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="D27" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="E27" s="17">
-        <v>18</v>
-      </c>
-      <c r="F27" s="17">
-        <v>450</v>
-      </c>
-      <c r="G27" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="H27" s="12"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
-      <c r="K27" s="1"/>
-      <c r="L27" s="1"/>
-    </row>
-    <row r="28" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="B28" s="18">
-        <v>20</v>
-      </c>
-      <c r="C28" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="D28" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="E28" s="19">
-        <v>1</v>
-      </c>
-      <c r="F28" s="19">
-        <v>15</v>
-      </c>
-      <c r="G28" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="H28" s="13"/>
-    </row>
-    <row r="29" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="31"/>
-      <c r="B29" s="22">
-        <v>21</v>
-      </c>
-      <c r="C29" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="D29" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="E29" s="21">
-        <v>1</v>
-      </c>
-      <c r="F29" s="21">
-        <v>15</v>
-      </c>
-      <c r="G29" s="21" t="s">
-        <v>56</v>
+      <c r="G28" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="H28" s="10"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+    </row>
+    <row r="29" spans="1:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="32"/>
+      <c r="B29" s="16">
+        <v>23</v>
+      </c>
+      <c r="C29" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D29" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E29" s="17">
+        <v>1</v>
+      </c>
+      <c r="F29" s="17">
+        <v>25</v>
+      </c>
+      <c r="G29" s="20" t="s">
+        <v>59</v>
       </c>
       <c r="H29" s="11"/>
     </row>
-    <row r="30" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="32" t="s">
-        <v>32</v>
-      </c>
+    <row r="30" spans="1:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="32"/>
       <c r="B30" s="16">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D30" s="17" t="s">
         <v>3</v>
@@ -1409,20 +1437,18 @@
       <c r="F30" s="17">
         <v>25</v>
       </c>
-      <c r="G30" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="H30" s="10"/>
-      <c r="I30" s="3"/>
-      <c r="J30" s="3"/>
-    </row>
-    <row r="31" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G30" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="H30" s="11"/>
+    </row>
+    <row r="31" spans="1:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="32"/>
       <c r="B31" s="16">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D31" s="17" t="s">
         <v>3</v>
@@ -1434,17 +1460,17 @@
         <v>25</v>
       </c>
       <c r="G31" s="20" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="H31" s="11"/>
     </row>
     <row r="32" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="32"/>
       <c r="B32" s="16">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C32" s="16" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D32" s="17" t="s">
         <v>3</v>
@@ -1456,39 +1482,39 @@
         <v>25</v>
       </c>
       <c r="G32" s="20" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H32" s="11"/>
     </row>
     <row r="33" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="32"/>
       <c r="B33" s="16">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C33" s="16" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D33" s="17" t="s">
         <v>3</v>
       </c>
       <c r="E33" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F33" s="17">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="G33" s="20" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="H33" s="11"/>
     </row>
     <row r="34" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="32"/>
       <c r="B34" s="16">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C34" s="16" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D34" s="17" t="s">
         <v>3</v>
@@ -1500,39 +1526,39 @@
         <v>25</v>
       </c>
       <c r="G34" s="20" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="H34" s="11"/>
     </row>
     <row r="35" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="32"/>
       <c r="B35" s="16">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C35" s="16" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D35" s="17" t="s">
         <v>3</v>
       </c>
       <c r="E35" s="17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F35" s="17">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="G35" s="20" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H35" s="11"/>
     </row>
-    <row r="36" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="32"/>
       <c r="B36" s="16">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C36" s="16" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D36" s="17" t="s">
         <v>3</v>
@@ -1544,86 +1570,42 @@
         <v>25</v>
       </c>
       <c r="G36" s="20" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="H36" s="11"/>
     </row>
-    <row r="37" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="32"/>
-      <c r="B37" s="16">
-        <v>29</v>
-      </c>
-      <c r="C37" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="D37" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="E37" s="17">
-        <v>1</v>
-      </c>
-      <c r="F37" s="17">
+    <row r="37" spans="1:8" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="33"/>
+      <c r="B37" s="23">
+        <v>31</v>
+      </c>
+      <c r="C37" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="D37" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E37" s="14">
+        <v>1</v>
+      </c>
+      <c r="F37" s="14">
         <v>25</v>
       </c>
-      <c r="G37" s="20" t="s">
-        <v>64</v>
+      <c r="G37" s="14" t="s">
+        <v>66</v>
       </c>
       <c r="H37" s="11"/>
     </row>
-    <row r="38" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="32"/>
-      <c r="B38" s="16">
-        <v>30</v>
-      </c>
-      <c r="C38" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="D38" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="E38" s="17">
-        <v>1</v>
-      </c>
-      <c r="F38" s="17">
-        <v>25</v>
-      </c>
-      <c r="G38" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="H38" s="11"/>
-    </row>
-    <row r="39" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="33"/>
-      <c r="B39" s="23">
-        <v>31</v>
-      </c>
-      <c r="C39" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="D39" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="E39" s="14">
-        <v>1</v>
-      </c>
-      <c r="F39" s="14">
-        <v>25</v>
-      </c>
-      <c r="G39" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="H39" s="11"/>
-    </row>
-    <row r="40" spans="1:8" ht="9" customHeight="1" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="38" spans="1:8" ht="9" customHeight="1" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="A1:G6"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="A30:A39"/>
-    <mergeCell ref="A9:A17"/>
-    <mergeCell ref="A18:A23"/>
+    <mergeCell ref="A1:G4"/>
     <mergeCell ref="A26:A27"/>
+    <mergeCell ref="A28:A37"/>
+    <mergeCell ref="A7:A15"/>
+    <mergeCell ref="A16:A21"/>
     <mergeCell ref="A24:A25"/>
+    <mergeCell ref="A22:A23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>